<commit_message>
Update Domain Model & Risk List. Add the various scripts used in creating the test database for future information and Add the TestDBModel for Compentency Test.
Signed-off-by: Jette McKellar <jette.mckellar@yahoo.com>
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Documents\ITC303-309\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Documents\ITC303-309\TeamPharmacon\pharmacy_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="138">
   <si>
     <t>Column</t>
   </si>
@@ -1317,6 +1317,32 @@
   </si>
   <si>
     <t>If team member is not committing changes on a regular basis, other team members are to remind member to do so.</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Application Metabase and vue.js do not meet project needs</t>
+  </si>
+  <si>
+    <t>New applications will need to be sourced</t>
+  </si>
+  <si>
+    <t>Schedule
+Technology
+Reliability of systems</t>
+  </si>
+  <si>
+    <t>Unable to execute required functions, such as visualisations</t>
+  </si>
+  <si>
+    <t>Difficulty in integrating software into project</t>
+  </si>
+  <si>
+    <t>Team members report issues immediately the arise</t>
+  </si>
+  <si>
+    <t>When indication start to appear that software is not compatible or doesn't work as desired, investigation starts urgently for new software to take its place</t>
   </si>
 </sst>
 </file>
@@ -2827,9 +2853,9 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3259,7 +3285,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>113</v>
       </c>
@@ -3343,23 +3369,47 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
+    <row r="15" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="E15" s="64" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F15" s="45"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="75"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="46"/>
+        <v>Yellow</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="I15" s="76" t="s">
+        <v>134</v>
+      </c>
+      <c r="J15" s="75" t="s">
+        <v>135</v>
+      </c>
+      <c r="K15" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="L15" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="M15" s="46" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="16" spans="1:21" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>

</xml_diff>

<commit_message>
Fixed small folder layout issues
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Documents\ITC303-309\TeamPharmacon\pharmacy_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Documents\ITC303-309\TeamPharmacon\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
   <si>
     <t>Column</t>
   </si>
@@ -1322,9 +1322,6 @@
     <t>6</t>
   </si>
   <si>
-    <t>Application Metabase and vue.js do not meet project needs</t>
-  </si>
-  <si>
     <t>New applications will need to be sourced</t>
   </si>
   <si>
@@ -1343,6 +1340,31 @@
   </si>
   <si>
     <t>When indication start to appear that software is not compatible or doesn't work as desired, investigation starts urgently for new software to take its place</t>
+  </si>
+  <si>
+    <t>Ability of customised changes to error entry form to flow through to database automatically</t>
+  </si>
+  <si>
+    <t>A main feature of the application will not be delivered</t>
+  </si>
+  <si>
+    <t>Feasibility
+Overall project failure</t>
+  </si>
+  <si>
+    <t>Unable to have the MySQL database automatically update to reflect changes made to the error entry form</t>
+  </si>
+  <si>
+    <t>In ability to solve issue</t>
+  </si>
+  <si>
+    <t>May need to remove flexibility from application.</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Applications Metabase and vue.js do not meet project needs</t>
   </si>
 </sst>
 </file>
@@ -2853,9 +2875,9 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3202,48 +3224,48 @@
       </c>
     </row>
     <row r="11" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="E11" s="64" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F11" s="44" t="s">
-        <v>97</v>
+      <c r="F11" s="45" t="s">
+        <v>144</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="I11" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="J11" s="76" t="s">
-        <v>99</v>
+        <v>133</v>
+      </c>
+      <c r="J11" s="75" t="s">
+        <v>134</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="L11" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="M11" s="77" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="78" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="M11" s="46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="78" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>104</v>
       </c>
@@ -3254,35 +3276,35 @@
         <v>59</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E12" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v>Yellow</v>
+        <f>IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="High"),AND(B12&lt;&gt;"Closed",C12="High",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Low",D12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",C12="Medium",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
+        <v>Red</v>
       </c>
       <c r="F12" s="45" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="I12" s="76" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="J12" s="75" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="K12" s="71" t="s">
         <v>120</v>
       </c>
       <c r="L12" s="76" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="M12" s="46" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
@@ -3299,7 +3321,7 @@
         <v>60</v>
       </c>
       <c r="E13" s="64" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
         <v>Green</v>
       </c>
       <c r="F13" s="45" t="s">
@@ -3369,7 +3391,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" s="78" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>130</v>
       </c>
@@ -3377,57 +3399,81 @@
         <v>58</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E15" s="64" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(OR(AND(B15&lt;&gt;"Closed",C15="High",D15="High"),AND(B15&lt;&gt;"Closed",C15="High",D15="Medium"),AND(B15&lt;&gt;"Closed",C15="Medium",D15="High")),"Red",IF(OR(AND(B15&lt;&gt;"Closed",C15="High",D15="Low"),AND(B15&lt;&gt;"Closed",C15="Medium",D15="Medium"),AND(B15&lt;&gt;"Closed",C15="Low",D15="High")),"Yellow",IF(OR(AND(B15&lt;&gt;"Closed",C15="Medium",D15="Low"),AND(B15&lt;&gt;"Closed",C15="Low",D15="Low"),AND(B15&lt;&gt;"Closed",C15="Low",D15="Medium")),"Green",IF(B15="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
       <c r="F15" s="45" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="I15" s="76" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="J15" s="75" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="L15" s="76" t="s">
-        <v>136</v>
+        <v>111</v>
       </c>
       <c r="M15" s="46" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="61" t="s">
+        <v>60</v>
+      </c>
       <c r="E16" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="75"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="46"/>
+        <f>IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="High"),AND(B16&lt;&gt;"Closed",C16="High",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="High")),"Red",IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Low",D16="High")),"Yellow",IF(OR(AND(B16&lt;&gt;"Closed",C16="Medium",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Medium")),"Green",IF(B16="Closed","Closed",""))))</f>
+        <v>Yellow</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="J16" s="76" t="s">
+        <v>99</v>
+      </c>
+      <c r="K16" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="M16" s="77" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="17" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
@@ -3827,16 +3873,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:D35 C7:D12">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H35 H7:H12">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B35 B7:B12">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K35 K7:K12">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Pharmacy Error Tracker Risk List and Project Plan - Pharmacy Error Tracker revised and updated. Inception Phase Status Assessment completed. Elaboration Iteration Plan 1 completed. 20180413 - Meeting Minutes completed.
Signed-off-by: Jette McKellar <jette.mckellar@yahoo.com>
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Documents\ITC303-309\TeamPharmacon\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risk_Tracking_Log!$B$6:$D$6</definedName>
     <definedName name="as">[1]DropDown_Elements!$A$2:$A$30</definedName>
     <definedName name="OLE_LINK1" localSheetId="1">Risk_Tracking_Log!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$36</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="153">
   <si>
     <t>Column</t>
   </si>
@@ -1355,9 +1355,6 @@
     <t>Unable to have the MySQL database automatically update to reflect changes made to the error entry form</t>
   </si>
   <si>
-    <t>In ability to solve issue</t>
-  </si>
-  <si>
     <t>May need to remove flexibility from application.</t>
   </si>
   <si>
@@ -1365,6 +1362,34 @@
   </si>
   <si>
     <t>Applications Metabase and vue.js do not meet project needs</t>
+  </si>
+  <si>
+    <t>Team members not being able to test developments on local machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changes to application made by individual members will need to be pushed to remote server for testing. </t>
+  </si>
+  <si>
+    <t>Schedule
+Reliability of System</t>
+  </si>
+  <si>
+    <t>Overall application development becomes buggy and unreliable due to untested code being implemented</t>
+  </si>
+  <si>
+    <t>Inability to solve issue</t>
+  </si>
+  <si>
+    <t>Currently team members do not have local testing environments</t>
+  </si>
+  <si>
+    <t>Guide to be created during Elaboration Iteration 1 to provide details on implementation of local testing environment</t>
+  </si>
+  <si>
+    <t>Team meeting where individual members are provided step-by-step instruction during meeting to implement local environment.</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -2872,12 +2897,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U36"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3195,7 +3220,7 @@
         <v>60</v>
       </c>
       <c r="E10" s="64" t="str">
-        <f t="shared" ref="E10:E35" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
+        <f t="shared" ref="E10:E36" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
       <c r="F10" s="74" t="s">
@@ -3223,7 +3248,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>96</v>
       </c>
@@ -3231,41 +3256,41 @@
         <v>58</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>69</v>
       </c>
       <c r="E11" s="64" t="str">
         <f>IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
-        <v>Yellow</v>
+        <v>Red</v>
       </c>
       <c r="F11" s="45" t="s">
         <v>144</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="I11" s="76" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="J11" s="75" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="K11" s="71" t="s">
         <v>66</v>
       </c>
       <c r="L11" s="76" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="M11" s="46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="78" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>104</v>
       </c>
@@ -3273,41 +3298,41 @@
         <v>58</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="64" t="str">
         <f>IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="High"),AND(B12&lt;&gt;"Closed",C12="High",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Low",D12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",C12="Medium",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
-        <v>Red</v>
+        <v>Yellow</v>
       </c>
       <c r="F12" s="45" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="I12" s="76" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="J12" s="75" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="K12" s="71" t="s">
-        <v>120</v>
+        <v>66</v>
       </c>
       <c r="L12" s="76" t="s">
         <v>135</v>
       </c>
       <c r="M12" s="46" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="78" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>113</v>
       </c>
@@ -3315,41 +3340,41 @@
         <v>58</v>
       </c>
       <c r="C13" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>60</v>
       </c>
       <c r="E13" s="64" t="str">
         <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
-        <v>Green</v>
+        <v>Red</v>
       </c>
       <c r="F13" s="45" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="I13" s="76" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="J13" s="75" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="K13" s="71" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="L13" s="76" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="M13" s="46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>123</v>
       </c>
@@ -3363,79 +3388,79 @@
         <v>60</v>
       </c>
       <c r="E14" s="64" t="str">
+        <f>IF(OR(AND(B14&lt;&gt;"Closed",C14="High",D14="High"),AND(B14&lt;&gt;"Closed",C14="High",D14="Medium"),AND(B14&lt;&gt;"Closed",C14="Medium",D14="High")),"Red",IF(OR(AND(B14&lt;&gt;"Closed",C14="High",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Medium",D14="Medium"),AND(B14&lt;&gt;"Closed",C14="Low",D14="High")),"Yellow",IF(OR(AND(B14&lt;&gt;"Closed",C14="Medium",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Low",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Low",D14="Medium")),"Green",IF(B14="Closed","Closed",""))))</f>
+        <v>Green</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" s="75" t="s">
+        <v>119</v>
+      </c>
+      <c r="K14" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="76" t="s">
+        <v>121</v>
+      </c>
+      <c r="M14" s="46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="64" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F15" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G15" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="H14" s="41" t="s">
+      <c r="H15" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="I14" s="76" t="s">
+      <c r="I15" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="J14" s="76" t="s">
+      <c r="J15" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="K14" s="71" t="s">
+      <c r="K15" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="L14" s="76" t="s">
+      <c r="L15" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="M14" s="46" t="s">
+      <c r="M15" s="46" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="78" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="64" t="str">
-        <f>IF(OR(AND(B15&lt;&gt;"Closed",C15="High",D15="High"),AND(B15&lt;&gt;"Closed",C15="High",D15="Medium"),AND(B15&lt;&gt;"Closed",C15="Medium",D15="High")),"Red",IF(OR(AND(B15&lt;&gt;"Closed",C15="High",D15="Low"),AND(B15&lt;&gt;"Closed",C15="Medium",D15="Medium"),AND(B15&lt;&gt;"Closed",C15="Low",D15="High")),"Yellow",IF(OR(AND(B15&lt;&gt;"Closed",C15="Medium",D15="Low"),AND(B15&lt;&gt;"Closed",C15="Low",D15="Low"),AND(B15&lt;&gt;"Closed",C15="Low",D15="Medium")),"Green",IF(B15="Closed","Closed",""))))</f>
-        <v>Yellow</v>
-      </c>
-      <c r="F15" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="I15" s="76" t="s">
-        <v>108</v>
-      </c>
-      <c r="J15" s="75" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="L15" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="M15" s="46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>143</v>
+    <row r="16" spans="1:21" s="78" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>58</v>
@@ -3443,55 +3468,79 @@
       <c r="C16" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="27" t="s">
         <v>60</v>
       </c>
       <c r="E16" s="64" t="str">
         <f>IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="High"),AND(B16&lt;&gt;"Closed",C16="High",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="High")),"Red",IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Low",D16="High")),"Yellow",IF(OR(AND(B16&lt;&gt;"Closed",C16="Medium",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Medium")),"Green",IF(B16="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="76" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="K16" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="L16" s="76" t="s">
+        <v>111</v>
+      </c>
+      <c r="M16" s="46" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="64" t="str">
+        <f>IF(OR(AND(B17&lt;&gt;"Closed",C17="High",D17="High"),AND(B17&lt;&gt;"Closed",C17="High",D17="Medium"),AND(B17&lt;&gt;"Closed",C17="Medium",D17="High")),"Red",IF(OR(AND(B17&lt;&gt;"Closed",C17="High",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Medium",D17="Medium"),AND(B17&lt;&gt;"Closed",C17="Low",D17="High")),"Yellow",IF(OR(AND(B17&lt;&gt;"Closed",C17="Medium",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Low",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Low",D17="Medium")),"Green",IF(B17="Closed","Closed",""))))</f>
+        <v>Yellow</v>
+      </c>
+      <c r="F17" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="G17" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H17" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="I16" s="76" t="s">
+      <c r="I17" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="76" t="s">
+      <c r="J17" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="K16" s="71" t="s">
+      <c r="K17" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="L16" s="76" t="s">
+      <c r="L17" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="M16" s="77" t="s">
+      <c r="M17" s="77" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="75"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="46"/>
     </row>
     <row r="18" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
@@ -3799,38 +3848,56 @@
       <c r="L34" s="76"/>
       <c r="M34" s="46"/>
     </row>
-    <row r="35" spans="1:13" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="15" t="str">
+    <row r="35" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="12"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="64" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="48"/>
-    </row>
-    <row r="36" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="41"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="76"/>
+      <c r="M35" s="46"/>
+    </row>
+    <row r="36" spans="1:13" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F36" s="47"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="70"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="48"/>
+    </row>
+    <row r="37" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:D6"/>
@@ -3839,7 +3906,7 @@
     <mergeCell ref="J5:L5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C36:E65536 C1:E1 B6:C6 B7:B35">
+  <conditionalFormatting sqref="C37:E65537 C1:E1 B6:C6 B7:B36">
     <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -3850,7 +3917,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E35">
+  <conditionalFormatting sqref="E7:E36">
     <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
@@ -3861,7 +3928,7 @@
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D35">
+  <conditionalFormatting sqref="C7:D36">
     <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -3873,16 +3940,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:D35 C7:D12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:D36 C7:D12">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H35 H7:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H36 H7:H12">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B35 B7:B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B36 B7:B12">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K35 K7:K12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K36 K7:K12">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update to Risk List
Signed-off-by: Jette McKellar <jette.mckellar@yahoo.com>
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jette\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITC303\Clone\pharmacy_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="161">
   <si>
     <t>Column</t>
   </si>
@@ -1390,6 +1390,30 @@
   </si>
   <si>
     <t>8</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>May not pickup application errors if not done</t>
+  </si>
+  <si>
+    <t>Unit &amp; integration testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigation into unit &amp; integration testing within Vue.js is confusing and hard to follow. </t>
+  </si>
+  <si>
+    <t>Unable to create necessary tests for the use cases</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Decided that due to confusion of available documentation, UAT testing is to be done in a more thorough way to ensure errors are found and fixed</t>
+  </si>
+  <si>
+    <t>Thorough UAT testing</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2276,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2317,7 +2363,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2900,9 +2951,9 @@
   <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3295,7 +3346,7 @@
         <v>104</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>69</v>
@@ -3305,7 +3356,7 @@
       </c>
       <c r="E12" s="64" t="str">
         <f>IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="High"),AND(B12&lt;&gt;"Closed",C12="High",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Low",D12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",C12="Medium",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F12" s="45" t="s">
         <v>143</v>
@@ -3337,7 +3388,7 @@
         <v>113</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>59</v>
@@ -3347,7 +3398,7 @@
       </c>
       <c r="E13" s="64" t="str">
         <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
-        <v>Red</v>
+        <v>Closed</v>
       </c>
       <c r="F13" s="45" t="s">
         <v>137</v>
@@ -3542,23 +3593,47 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
+    <row r="18" spans="1:13" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>69</v>
+      </c>
       <c r="E18" s="64" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="46"/>
+        <v>Closed</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="76" t="s">
+        <v>156</v>
+      </c>
+      <c r="J18" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="L18" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="M18" s="46" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="19" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
@@ -3907,35 +3982,35 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C37:E65537 C1:E1 B6:C6 B7:B36">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E36">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D36">
-    <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated Risk List - update to status of existing risks.
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITC303\Clone\pharmacy_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan Smith\Desktop\itc303thebestteam\pharmacy_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7005" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -24,11 +24,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risk_Tracking_Log!$B$6:$D$6</definedName>
     <definedName name="as">[1]DropDown_Elements!$A$2:$A$30</definedName>
     <definedName name="OLE_LINK1" localSheetId="1">Risk_Tracking_Log!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$33</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
   <si>
     <t>Column</t>
   </si>
@@ -1033,90 +1033,7 @@
     <t>Low</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">EXAMPLE: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Current project skill set may not be adequate to complete all project work.  The current development team has been working in a Windows 2k environment, and the current requirements are for a LINUX environment.  The project schedule would require 1500 development hours of a skilled LINUX operator, and approximately 1900 to 2200 if we retrain our current resources.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>EXAMPLE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> If required skills are not identified or obtained, project schedule may slip and possibly restrict the accomplishment of project goals.</t>
-    </r>
-  </si>
-  <si>
-    <t>Project Resources
-Budget
-Schedule</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">EXAMPLE: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Schedule approaches the required start date with no identification of required skill sets.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>EXAMPLE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Four weeks prior to scheduled start date if no resource is identified with required skill set implement contingency plan.</t>
-    </r>
-  </si>
-  <si>
     <t>Mitigation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">EXAMPLE: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Find internal resource that meets required skill set or train existing resources on LINUX.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>EXAMPLE:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Find resource that meets required skill set through external hiring sources.</t>
-    </r>
   </si>
   <si>
     <t>Medium</t>
@@ -1394,32 +1311,11 @@
   <si>
     <t>Closed</t>
   </si>
-  <si>
-    <t>May not pickup application errors if not done</t>
-  </si>
-  <si>
-    <t>Unit &amp; integration testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investigation into unit &amp; integration testing within Vue.js is confusing and hard to follow. </t>
-  </si>
-  <si>
-    <t>Unable to create necessary tests for the use cases</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Decided that due to confusion of available documentation, UAT testing is to be done in a more thorough way to ensure errors are found and fixed</t>
-  </si>
-  <si>
-    <t>Thorough UAT testing</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -1545,7 +1441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1807,19 +1703,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1927,21 +1810,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -2020,7 +1888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2143,93 +2011,78 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2241,17 +2094,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2276,29 +2129,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -2363,12 +2194,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2770,14 +2596,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="81" t="str">
+      <c r="A1" s="76" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="82"/>
+      <c r="B1" s="77"/>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -2800,7 +2626,7 @@
       <c r="A5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="48" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2808,7 +2634,7 @@
       <c r="A6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="48" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2816,7 +2642,7 @@
       <c r="A7" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="48" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2824,7 +2650,7 @@
       <c r="A8" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="49" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2832,7 +2658,7 @@
       <c r="A9" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="48" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2840,7 +2666,7 @@
       <c r="A10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="48" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2848,7 +2674,7 @@
       <c r="A11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="48" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2856,7 +2682,7 @@
       <c r="A12" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="48" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2864,7 +2690,7 @@
       <c r="A13" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="48" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2872,7 +2698,7 @@
       <c r="A14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="48" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2880,7 +2706,7 @@
       <c r="A15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="48" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2888,15 +2714,15 @@
       <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="48" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="64" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2948,12 +2774,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U37"/>
+  <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2963,11 +2789,11 @@
     <col min="3" max="3" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="34" style="49" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.85546875" style="49" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="49" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.85546875" style="49" customWidth="1"/>
+    <col min="6" max="7" width="34" style="47" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.85546875" style="47" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="30.85546875" style="47" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="4"/>
     <col min="15" max="15" width="6" style="4" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="4"/>
@@ -3014,16 +2840,16 @@
         <v>Pharmacy Error Tracker</v>
       </c>
       <c r="K2" s="38"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -3047,16 +2873,16 @@
         <v>CSU</v>
       </c>
       <c r="K3" s="38"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="66"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62"/>
+      <c r="N3" s="62"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="62"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="62"/>
+      <c r="T3" s="62"/>
+      <c r="U3" s="62"/>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -3080,16 +2906,16 @@
         <v>James Tulip</v>
       </c>
       <c r="K4" s="38"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
-      <c r="U4" s="66"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
     </row>
     <row r="5" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
@@ -3097,76 +2923,78 @@
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="40"/>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="9" t="str">
         <f>A5</f>
         <v>Project Description:</v>
       </c>
-      <c r="J5" s="85" t="str">
+      <c r="J5" s="80" t="str">
         <f>D5</f>
         <v>Creation of a single page mobile web application</v>
       </c>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="66"/>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
     </row>
     <row r="6" spans="1:21" s="3" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="55" t="s">
+      <c r="G6" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="53" t="s">
+      <c r="K6" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="L6" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="M6" s="65" t="s">
+      <c r="M6" s="61" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="101.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+    <row r="7" spans="1:21" s="73" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>63</v>
+      </c>
       <c r="B7" s="14" t="s">
         <v>58</v>
       </c>
@@ -3176,803 +3004,685 @@
       <c r="D7" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="64" t="str">
-        <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
+      <c r="E7" s="60" t="str">
+        <f t="shared" ref="E7:E33" si="0">IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="70" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="L7" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="M7" s="72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="73" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="J7" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L7" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="M7" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="O7" s="4" t="str">
-        <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="High"), AND(B7&lt;&gt;"Closed",C7="High", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",E7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Medium", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",E7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Low", E7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",E7="Medium")),"Green","")))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="64" t="str">
+      <c r="E8" s="60" t="str">
         <f>IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
-        <v>Yellow</v>
-      </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="43"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+        <v>Closed</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="I8" s="71" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="M8" s="44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="B9" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="64" t="str">
+      <c r="E9" s="60" t="str">
         <f>IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="High"),AND(B9&lt;&gt;"Closed",C9="High",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="High")),"Red",IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Low",D9="High")),"Yellow",IF(OR(AND(B9&lt;&gt;"Closed",C9="Medium",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Medium")),"Green",IF(B9="Closed","Closed",""))))</f>
         <v>Green</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="43"/>
-    </row>
-    <row r="10" spans="1:21" s="78" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>70</v>
+      <c r="F9" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="J9" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="73" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>58</v>
+        <v>146</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="64" t="str">
-        <f t="shared" ref="E10:E36" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
-        <v>Yellow</v>
-      </c>
-      <c r="F10" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="75" t="s">
-        <v>72</v>
+        <v>62</v>
+      </c>
+      <c r="E10" s="60" t="str">
+        <f>IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
+        <v>Closed</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>131</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="76" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="75" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L10" s="76" t="s">
-        <v>76</v>
-      </c>
-      <c r="M10" s="77" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="70" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="L10" s="71" t="s">
+        <v>128</v>
+      </c>
+      <c r="M10" s="44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="64" t="str">
+        <v>60</v>
+      </c>
+      <c r="E11" s="60" t="str">
         <f>IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
-        <v>Red</v>
-      </c>
-      <c r="F11" s="45" t="s">
-        <v>144</v>
+        <v>Green</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>107</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>146</v>
-      </c>
-      <c r="I11" s="76" t="s">
-        <v>147</v>
-      </c>
-      <c r="J11" s="75" t="s">
-        <v>149</v>
-      </c>
-      <c r="K11" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L11" s="76" t="s">
-        <v>150</v>
-      </c>
-      <c r="M11" s="46" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="I11" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="K11" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="73" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="64" t="str">
-        <f>IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="High"),AND(B12&lt;&gt;"Closed",C12="High",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="High")),"Red",IF(OR(AND(B12&lt;&gt;"Closed",C12="High",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Medium",D12="Medium"),AND(B12&lt;&gt;"Closed",C12="Low",D12="High")),"Yellow",IF(OR(AND(B12&lt;&gt;"Closed",C12="Medium",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Low"),AND(B12&lt;&gt;"Closed",C12="Low",D12="Medium")),"Green",IF(B12="Closed","Closed",""))))</f>
-        <v>Closed</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>143</v>
+        <v>60</v>
+      </c>
+      <c r="E12" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v>Green</v>
+      </c>
+      <c r="F12" s="43" t="s">
+        <v>117</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="I12" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="J12" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="K12" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L12" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="71" t="s">
+        <v>121</v>
+      </c>
+      <c r="J12" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="73" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="M12" s="46" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="78" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>113</v>
-      </c>
       <c r="B13" s="14" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="64" t="str">
+        <v>60</v>
+      </c>
+      <c r="E13" s="60" t="str">
         <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
-        <v>Closed</v>
-      </c>
-      <c r="F13" s="45" t="s">
-        <v>137</v>
+        <v>Yellow</v>
+      </c>
+      <c r="F13" s="43" t="s">
+        <v>98</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="I13" s="76" t="s">
-        <v>140</v>
-      </c>
-      <c r="J13" s="75" t="s">
-        <v>148</v>
-      </c>
-      <c r="K13" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="L13" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="M13" s="46" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>123</v>
+        <v>110</v>
+      </c>
+      <c r="I13" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="J13" s="70" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="64" t="str">
+      <c r="E14" s="60" t="str">
         <f>IF(OR(AND(B14&lt;&gt;"Closed",C14="High",D14="High"),AND(B14&lt;&gt;"Closed",C14="High",D14="Medium"),AND(B14&lt;&gt;"Closed",C14="Medium",D14="High")),"Red",IF(OR(AND(B14&lt;&gt;"Closed",C14="High",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Medium",D14="Medium"),AND(B14&lt;&gt;"Closed",C14="Low",D14="High")),"Yellow",IF(OR(AND(B14&lt;&gt;"Closed",C14="Medium",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Low",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Low",D14="Medium")),"Green",IF(B14="Closed","Closed",""))))</f>
-        <v>Green</v>
-      </c>
-      <c r="F14" s="45" t="s">
-        <v>114</v>
+        <v>Yellow</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>90</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>116</v>
-      </c>
-      <c r="I14" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="J14" s="75" t="s">
-        <v>119</v>
-      </c>
-      <c r="K14" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L14" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="M14" s="46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="64" t="str">
+        <v>91</v>
+      </c>
+      <c r="I14" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="60" t="str">
         <f t="shared" si="0"/>
-        <v>Green</v>
-      </c>
-      <c r="F15" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="J15" s="76" t="s">
-        <v>127</v>
-      </c>
-      <c r="K15" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L15" s="76" t="s">
-        <v>110</v>
-      </c>
-      <c r="M15" s="46" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="78" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="64" t="str">
-        <f>IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="High"),AND(B16&lt;&gt;"Closed",C16="High",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="High")),"Red",IF(OR(AND(B16&lt;&gt;"Closed",C16="High",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Medium",D16="Medium"),AND(B16&lt;&gt;"Closed",C16="Low",D16="High")),"Yellow",IF(OR(AND(B16&lt;&gt;"Closed",C16="Medium",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Low"),AND(B16&lt;&gt;"Closed",C16="Low",D16="Medium")),"Green",IF(B16="Closed","Closed",""))))</f>
-        <v>Yellow</v>
-      </c>
-      <c r="F16" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="G16" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="I16" s="76" t="s">
-        <v>108</v>
-      </c>
-      <c r="J16" s="75" t="s">
-        <v>109</v>
-      </c>
-      <c r="K16" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="L16" s="76" t="s">
-        <v>111</v>
-      </c>
-      <c r="M16" s="46" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="78" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="64" t="str">
-        <f>IF(OR(AND(B17&lt;&gt;"Closed",C17="High",D17="High"),AND(B17&lt;&gt;"Closed",C17="High",D17="Medium"),AND(B17&lt;&gt;"Closed",C17="Medium",D17="High")),"Red",IF(OR(AND(B17&lt;&gt;"Closed",C17="High",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Medium",D17="Medium"),AND(B17&lt;&gt;"Closed",C17="Low",D17="High")),"Yellow",IF(OR(AND(B17&lt;&gt;"Closed",C17="Medium",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Low",D17="Low"),AND(B17&lt;&gt;"Closed",C17="Low",D17="Medium")),"Green",IF(B17="Closed","Closed",""))))</f>
-        <v>Yellow</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" s="41" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="J17" s="76" t="s">
-        <v>99</v>
-      </c>
-      <c r="K17" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="L17" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="M17" s="77" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="64" t="str">
+        <v/>
+      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="44"/>
+    </row>
+    <row r="16" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="60" t="str">
         <f t="shared" si="0"/>
-        <v>Closed</v>
-      </c>
-      <c r="F18" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="I18" s="76" t="s">
-        <v>156</v>
-      </c>
-      <c r="J18" s="75" t="s">
-        <v>157</v>
-      </c>
-      <c r="K18" s="71" t="s">
-        <v>66</v>
-      </c>
-      <c r="L18" s="76" t="s">
-        <v>159</v>
-      </c>
-      <c r="M18" s="46" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+        <v/>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="44"/>
+    </row>
+    <row r="17" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="44"/>
+    </row>
+    <row r="18" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="F18" s="43"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="44"/>
+    </row>
+    <row r="19" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="14"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="64" t="str">
+      <c r="E19" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F19" s="45"/>
+      <c r="F19" s="43"/>
       <c r="G19" s="41"/>
       <c r="H19" s="41"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="46"/>
-    </row>
-    <row r="20" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I19" s="71"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="44"/>
+    </row>
+    <row r="20" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="14"/>
       <c r="C20" s="27"/>
       <c r="D20" s="27"/>
-      <c r="E20" s="64" t="str">
+      <c r="E20" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F20" s="45"/>
+      <c r="F20" s="43"/>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="75"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="46"/>
-    </row>
-    <row r="21" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I20" s="71"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="44"/>
+    </row>
+    <row r="21" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="14"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
-      <c r="E21" s="64" t="str">
+      <c r="E21" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F21" s="45"/>
+      <c r="F21" s="43"/>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="46"/>
-    </row>
-    <row r="22" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I21" s="71"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="44"/>
+    </row>
+    <row r="22" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="14"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
-      <c r="E22" s="64" t="str">
+      <c r="E22" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="43"/>
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="46"/>
-    </row>
-    <row r="23" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I22" s="71"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="44"/>
+    </row>
+    <row r="23" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="14"/>
       <c r="C23" s="27"/>
       <c r="D23" s="27"/>
-      <c r="E23" s="64" t="str">
+      <c r="E23" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F23" s="45"/>
+      <c r="F23" s="43"/>
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="46"/>
-    </row>
-    <row r="24" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="71"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="44"/>
+    </row>
+    <row r="24" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="64" t="str">
+      <c r="E24" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F24" s="45"/>
+      <c r="F24" s="43"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="46"/>
-    </row>
-    <row r="25" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I24" s="71"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="44"/>
+    </row>
+    <row r="25" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="14"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
-      <c r="E25" s="64" t="str">
+      <c r="E25" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F25" s="45"/>
+      <c r="F25" s="43"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
-      <c r="I25" s="76"/>
-      <c r="J25" s="75"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="46"/>
-    </row>
-    <row r="26" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I25" s="71"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="44"/>
+    </row>
+    <row r="26" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="14"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="64" t="str">
+      <c r="E26" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F26" s="45"/>
+      <c r="F26" s="43"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="46"/>
-    </row>
-    <row r="27" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I26" s="71"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="71"/>
+      <c r="M26" s="44"/>
+    </row>
+    <row r="27" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="14"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
-      <c r="E27" s="64" t="str">
+      <c r="E27" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F27" s="45"/>
+      <c r="F27" s="43"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="46"/>
-    </row>
-    <row r="28" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I27" s="71"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="44"/>
+    </row>
+    <row r="28" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="14"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
-      <c r="E28" s="64" t="str">
+      <c r="E28" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F28" s="45"/>
+      <c r="F28" s="43"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="75"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="46"/>
-    </row>
-    <row r="29" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I28" s="71"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="44"/>
+    </row>
+    <row r="29" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="14"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
-      <c r="E29" s="64" t="str">
+      <c r="E29" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F29" s="45"/>
+      <c r="F29" s="43"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="75"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="46"/>
-    </row>
-    <row r="30" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I29" s="71"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="66"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="44"/>
+    </row>
+    <row r="30" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12"/>
       <c r="B30" s="14"/>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
-      <c r="E30" s="64" t="str">
+      <c r="E30" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F30" s="45"/>
+      <c r="F30" s="43"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="75"/>
-      <c r="K30" s="71"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="46"/>
-    </row>
-    <row r="31" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I30" s="71"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="44"/>
+    </row>
+    <row r="31" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="12"/>
       <c r="B31" s="14"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="64" t="str">
+      <c r="E31" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F31" s="45"/>
+      <c r="F31" s="43"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="75"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="46"/>
-    </row>
-    <row r="32" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I31" s="71"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="44"/>
+    </row>
+    <row r="32" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12"/>
       <c r="B32" s="14"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="64" t="str">
+      <c r="E32" s="60" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F32" s="45"/>
+      <c r="F32" s="43"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="46"/>
-    </row>
-    <row r="33" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="64" t="str">
+      <c r="I32" s="71"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="44"/>
+    </row>
+    <row r="33" spans="1:13" s="73" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F33" s="45"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="76"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="74"/>
       <c r="J33" s="75"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="76"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="74"/>
       <c r="M33" s="46"/>
     </row>
-    <row r="34" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F34" s="45"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="76"/>
-      <c r="M34" s="46"/>
-    </row>
-    <row r="35" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="64" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F35" s="45"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="46"/>
-    </row>
-    <row r="36" spans="1:13" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="79"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="70"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="48"/>
-    </row>
-    <row r="37" spans="1:13" s="78" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
+    <row r="34" spans="1:13" s="73" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
     </row>
   </sheetData>
   <autoFilter ref="B6:D6"/>
@@ -3981,50 +3691,50 @@
     <mergeCell ref="J5:L5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C37:E65537 C1:E1 B6:C6 B7:B36">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C34:E65534 C1:E1 B6:C6 B7:B33">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E36">
-    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="E7:E33">
+    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D36">
-    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="C7:D33">
+    <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:D36 C7:D12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D33">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H36 H7:H12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H33">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B36 B7:B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B33">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K13:K36 K7:K12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K33">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4051,103 +3761,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="54" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="55" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="55" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="55" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="55" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="55" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="55" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="57" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="55" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="57" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="55" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="55" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="55" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="55" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="57" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="57" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="57" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="57" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Risk List for LCAM resubmission.
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan Smith\Desktop\itc303thebestteam\pharmacy_app\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan Smith\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -555,7 +555,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="154">
   <si>
     <t>Column</t>
   </si>
@@ -1310,6 +1310,27 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>User Acceptence Tests not able to be written and completed on time in the same iteration as the use case implementations.</t>
+  </si>
+  <si>
+    <t>Construction phase delays to allow the completion of UATs.</t>
+  </si>
+  <si>
+    <t>UAT Tests not completed by the end of each iteration</t>
+  </si>
+  <si>
+    <t>UAT Tests not completed over a fornight after the previous iteration ended</t>
+  </si>
+  <si>
+    <t>Scheduling additional time for creating and completing UATs.</t>
+  </si>
+  <si>
+    <t>Adding an additional Contruction Phase iteration to act as a contingency for incomplete UAT testing, by reducing Transition Phase iteration duration from 14 days per iteration to 9 days.</t>
   </si>
 </sst>
 </file>
@@ -2779,7 +2800,7 @@
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3327,23 +3348,47 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
+    <row r="15" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>62</v>
+      </c>
       <c r="E15" s="60" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F15" s="43"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="70"/>
-      <c r="K15" s="66"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="44"/>
+        <v>Yellow</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="J15" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" s="71" t="s">
+        <v>152</v>
+      </c>
+      <c r="M15" s="44" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="16" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>

</xml_diff>

<commit_message>
Closed all risk items as they are no longer relevant to the project
</commit_message>
<xml_diff>
--- a/documents/Pharmacy Error Tracker Risk List.xlsx
+++ b/documents/Pharmacy Error Tracker Risk List.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan Smith\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITC309\App\pharmacy_app\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3EA64DEC-B811-4B00-BAAF-601C2E5ADCE1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7005" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7005" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -28,18 +29,18 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>eze3</author>
     <author>e</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -62,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -289,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0">
+    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -372,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -395,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0">
+    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -417,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -439,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="1" shapeId="0">
+    <comment ref="I6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -461,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0">
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -483,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="1" shapeId="0">
+    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -505,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0">
+    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -528,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0">
+    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -555,7 +556,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="153">
   <si>
     <t>Column</t>
   </si>
@@ -1024,9 +1025,6 @@
     <t>Contingency Plan</t>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
@@ -1336,7 +1334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -2150,7 +2148,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2215,7 +2235,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{F674ABE0-FB02-4CD2-947F-5ED4453F78EC}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2602,7 +2627,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2794,13 +2819,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3014,380 +3039,380 @@
     </row>
     <row r="7" spans="1:21" s="73" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="D7" s="27" t="s">
         <v>59</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>60</v>
       </c>
       <c r="E7" s="60" t="str">
         <f t="shared" ref="E7:E33" si="0">IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F7" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="70" t="s">
+      <c r="H7" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="I7" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="71" t="s">
+      <c r="J7" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="70" t="s">
+      <c r="K7" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" s="71" t="s">
+      <c r="M7" s="72" t="s">
         <v>69</v>
-      </c>
-      <c r="M7" s="72" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="73" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" s="60" t="str">
         <f>IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
         <v>Closed</v>
       </c>
       <c r="F8" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="H8" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="I8" s="71" t="s">
         <v>139</v>
       </c>
-      <c r="I8" s="71" t="s">
-        <v>140</v>
-      </c>
       <c r="J8" s="70" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="K8" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="71" t="s">
+      <c r="M8" s="44" t="s">
         <v>143</v>
-      </c>
-      <c r="M8" s="44" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="60" t="str">
         <f>IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="High"),AND(B9&lt;&gt;"Closed",C9="High",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="High")),"Red",IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Low",D9="High")),"Yellow",IF(OR(AND(B9&lt;&gt;"Closed",C9="Medium",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Medium")),"Green",IF(B9="Closed","Closed",""))))</f>
-        <v>Green</v>
+        <v>Closed</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G9" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="I9" s="71" t="s">
         <v>125</v>
       </c>
-      <c r="I9" s="71" t="s">
+      <c r="J9" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="J9" s="70" t="s">
+      <c r="K9" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="K9" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="71" t="s">
+      <c r="M9" s="44" t="s">
         <v>128</v>
-      </c>
-      <c r="M9" s="44" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="73" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="60" t="str">
         <f>IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
         <v>Closed</v>
       </c>
       <c r="F10" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="G10" s="41" t="s">
+      <c r="H10" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="H10" s="41" t="s">
+      <c r="I10" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="I10" s="71" t="s">
+      <c r="J10" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="K10" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="L10" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="M10" s="44" t="s">
         <v>133</v>
-      </c>
-      <c r="J10" s="70" t="s">
-        <v>141</v>
-      </c>
-      <c r="K10" s="66" t="s">
-        <v>113</v>
-      </c>
-      <c r="L10" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="M10" s="44" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="60" t="str">
         <f>IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="High"),AND(B11&lt;&gt;"Closed",C11="High",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="High")),"Red",IF(OR(AND(B11&lt;&gt;"Closed",C11="High",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Medium",D11="Medium"),AND(B11&lt;&gt;"Closed",C11="Low",D11="High")),"Yellow",IF(OR(AND(B11&lt;&gt;"Closed",C11="Medium",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Low"),AND(B11&lt;&gt;"Closed",C11="Low",D11="Medium")),"Green",IF(B11="Closed","Closed",""))))</f>
-        <v>Green</v>
+        <v>Closed</v>
       </c>
       <c r="F11" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="H11" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="41" t="s">
-        <v>109</v>
-      </c>
       <c r="I11" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="J11" s="70" t="s">
-        <v>112</v>
-      </c>
       <c r="K11" s="66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L11" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="M11" s="44" t="s">
         <v>114</v>
-      </c>
-      <c r="M11" s="44" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="73" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="60" t="str">
         <f t="shared" si="0"/>
-        <v>Green</v>
+        <v>Closed</v>
       </c>
       <c r="F12" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="H12" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="I12" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="K12" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="M12" s="44" t="s">
         <v>121</v>
-      </c>
-      <c r="J12" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="K12" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="44" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="73" customFormat="1" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="D13" s="27" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>60</v>
       </c>
       <c r="E13" s="60" t="str">
         <f>IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="High"),AND(B13&lt;&gt;"Closed",C13="High",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="High")),"Red",IF(OR(AND(B13&lt;&gt;"Closed",C13="High",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Medium",D13="Medium"),AND(B13&lt;&gt;"Closed",C13="Low",D13="High")),"Yellow",IF(OR(AND(B13&lt;&gt;"Closed",C13="Medium",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Low"),AND(B13&lt;&gt;"Closed",C13="Low",D13="Medium")),"Green",IF(B13="Closed","Closed",""))))</f>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="I13" s="71" t="s">
+      <c r="J13" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="J13" s="70" t="s">
-        <v>102</v>
-      </c>
       <c r="K13" s="66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L13" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="M13" s="44" t="s">
         <v>104</v>
-      </c>
-      <c r="M13" s="44" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="C14" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="D14" s="59" t="s">
         <v>59</v>
-      </c>
-      <c r="D14" s="59" t="s">
-        <v>60</v>
       </c>
       <c r="E14" s="60" t="str">
         <f>IF(OR(AND(B14&lt;&gt;"Closed",C14="High",D14="High"),AND(B14&lt;&gt;"Closed",C14="High",D14="Medium"),AND(B14&lt;&gt;"Closed",C14="Medium",D14="High")),"Red",IF(OR(AND(B14&lt;&gt;"Closed",C14="High",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Medium",D14="Medium"),AND(B14&lt;&gt;"Closed",C14="Low",D14="High")),"Yellow",IF(OR(AND(B14&lt;&gt;"Closed",C14="Medium",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Low",D14="Low"),AND(B14&lt;&gt;"Closed",C14="Low",D14="Medium")),"Green",IF(B14="Closed","Closed",""))))</f>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F14" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="G14" s="41" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" s="41" t="s">
+      <c r="I14" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" s="71" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="71" t="s">
+      <c r="K14" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="J14" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="K14" s="66" t="s">
+      <c r="L14" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="72" t="s">
         <v>94</v>
-      </c>
-      <c r="L14" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="M14" s="72" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="73" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="60" t="str">
         <f t="shared" si="0"/>
-        <v>Yellow</v>
+        <v>Closed</v>
       </c>
       <c r="F15" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="H15" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="71" t="s">
         <v>149</v>
       </c>
-      <c r="H15" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="71" t="s">
+      <c r="J15" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="J15" s="70" t="s">
+      <c r="K15" s="66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="71" t="s">
         <v>151</v>
       </c>
-      <c r="K15" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="L15" s="71" t="s">
+      <c r="M15" s="44" t="s">
         <v>152</v>
-      </c>
-      <c r="M15" s="44" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="73" customFormat="1" x14ac:dyDescent="0.2">
@@ -3730,56 +3755,56 @@
       <c r="M34" s="47"/>
     </row>
   </sheetData>
-  <autoFilter ref="B6:D6"/>
+  <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="2">
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="J5:L5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C34:E65534 C1:E1 B6:C6 B7:B33">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E33">
-    <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" stopIfTrue="1" operator="equal">
       <formula>"Yellow"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" stopIfTrue="1" operator="equal">
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:D33">
-    <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" stopIfTrue="1" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D33" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H33" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B33" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K33" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3793,7 +3818,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3812,97 +3837,97 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>